<commit_message>
Updated Walkthrough with Branching
</commit_message>
<xml_diff>
--- a/Walkthrough.xlsx
+++ b/Walkthrough.xlsx
@@ -4,21 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1.Setup for Collaboration" sheetId="1" r:id="rId1"/>
     <sheet name="2.Contribution to the project" sheetId="4" r:id="rId2"/>
     <sheet name="3.Added changes but need Revert" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="4.Branching" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>Requirement</t>
   </si>
@@ -483,13 +482,37 @@
   </si>
   <si>
     <t>User S added changes but needs to revert in the middle of the process</t>
+  </si>
+  <si>
+    <t>Req#</t>
+  </si>
+  <si>
+    <t>User S has been given a new urgent feature to accomplish. He needs to skip the main project and begin the new feature then merge the new feature into the main project.</t>
+  </si>
+  <si>
+    <t>touch newFeature.cs</t>
+  </si>
+  <si>
+    <t>Note: User S adds all codes for the new feature in his editor then saves the file.</t>
+  </si>
+  <si>
+    <t>git branch newBranch</t>
+  </si>
+  <si>
+    <t>git checkout newBranch</t>
+  </si>
+  <si>
+    <t>git checkout master</t>
+  </si>
+  <si>
+    <t>git merge newBranch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,6 +560,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -570,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -605,6 +635,26 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -908,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,7 +1384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
@@ -1526,26 +1576,77 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>4</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="27" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="28" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="29" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added WinMerge to excel file
</commit_message>
<xml_diff>
--- a/Walkthrough.xlsx
+++ b/Walkthrough.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1.Setup for Collaboration" sheetId="1" r:id="rId1"/>
     <sheet name="2.Contribution to the project" sheetId="4" r:id="rId2"/>
     <sheet name="3.Added changes but need Revert" sheetId="5" r:id="rId3"/>
     <sheet name="4.Branching" sheetId="3" r:id="rId4"/>
+    <sheet name="WinMerge" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>Requirement</t>
   </si>
@@ -506,13 +507,31 @@
   </si>
   <si>
     <t>git merge newBranch</t>
+  </si>
+  <si>
+    <t>User S needs to use WinMerge Tool to view differences in file versions.</t>
+  </si>
+  <si>
+    <t>git config diff.tool winmerge</t>
+  </si>
+  <si>
+    <t>Note: User S need to make sure that WinMerge is installed</t>
+  </si>
+  <si>
+    <t>Note: User S makes changes to some files in the working directory, then commits them all</t>
+  </si>
+  <si>
+    <t>git difftool HEAD HEAD~1 newClass.cs</t>
+  </si>
+  <si>
+    <t>Note : User S only wants to see the differences in the newClass.cs file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,6 +586,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -600,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -655,6 +681,18 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -958,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1384,7 +1422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
@@ -1578,12 +1616,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="29.5703125" customWidth="1"/>
     <col min="3" max="3" width="33.140625" customWidth="1"/>
     <col min="4" max="4" width="32.140625" customWidth="1"/>
@@ -1649,4 +1688,162 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20">
+        <v>5</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="22" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="1:4" s="22" customFormat="1" ht="63" x14ac:dyDescent="0.45">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="1:4" s="22" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="23"/>
+    </row>
+    <row r="6" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+    </row>
+    <row r="8" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+    </row>
+    <row r="10" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+    </row>
+    <row r="11" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+    </row>
+    <row r="12" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+    </row>
+    <row r="13" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+    </row>
+    <row r="14" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+    </row>
+    <row r="15" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+    </row>
+    <row r="16" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+    </row>
+    <row r="17" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+    </row>
+    <row r="18" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+    </row>
+    <row r="19" spans="1:4" s="22" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added config to walkthrough
</commit_message>
<xml_diff>
--- a/Walkthrough.xlsx
+++ b/Walkthrough.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="1.Setup for Collaboration" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>Requirement</t>
   </si>
@@ -525,6 +525,12 @@
   </si>
   <si>
     <t>Note : User S only wants to see the differences in the newClass.cs file</t>
+  </si>
+  <si>
+    <t>git config --global user.name "MyUserName"</t>
+  </si>
+  <si>
+    <t>git config --global user.email MyEmailAddress</t>
   </si>
 </sst>
 </file>
@@ -994,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,7 +1011,7 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="42.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="45.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="39" style="5" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1091,106 +1097,120 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+    <row r="13" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+    <row r="14" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="3" t="s">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+    <row r="17" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+    <row r="21" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="4" t="s">
+    <row r="22" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="4" t="s">
+    <row r="23" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="5" t="s">
+    <row r="24" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+    <row r="25" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
         <v>1</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B25" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1215,6 +1235,8 @@
     <row r="47" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1694,7 +1716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Commment About Commit Message
</commit_message>
<xml_diff>
--- a/Walkthrough.xlsx
+++ b/Walkthrough.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>Requirement</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Note: Files are uploaded and now tracking </t>
+    </r>
+    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -291,23 +294,59 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>git commit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> -m "Add work in progress solution files"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Note: Files are uploaded and now tracking </t>
-    </r>
+      <t xml:space="preserve">remote branch master </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>from Encrypter.</t>
+    </r>
+  </si>
+  <si>
+    <t>Note: Your branch is up-to-date with 'Encrypter/master'.</t>
+  </si>
+  <si>
+    <t>git log</t>
+  </si>
+  <si>
+    <t>Note:At any time you can type in git log to a) know the SHA1 hash of commits, b) Know the repo history , c) see all the comments for commits</t>
+  </si>
+  <si>
+    <t>Create a new to work in.  Change to that folder.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git clone </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://github.com/avinashbhujan/Encrypter.git</t>
+    </r>
+  </si>
+  <si>
+    <t>change to cloned folder which is the repository</t>
+  </si>
+  <si>
+    <t>Requirement met .  Collaboration can begin</t>
+  </si>
+  <si>
+    <t>Requirement met .  New test aded.  Committed. User G could get an update on his local repo</t>
+  </si>
+  <si>
+    <t>Note: to know which files have changed</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -317,57 +356,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">remote branch master </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>from Encrypter.</t>
-    </r>
-  </si>
-  <si>
-    <t>Note: Your branch is up-to-date with 'Encrypter/master'.</t>
-  </si>
-  <si>
-    <t>git log</t>
-  </si>
-  <si>
-    <t>Note:At any time you can type in git log to a) know the SHA1 hash of commits, b) Know the repo history , c) see all the comments for commits</t>
-  </si>
-  <si>
-    <t>Create a new to work in.  Change to that folder.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">git clone </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>https://github.com/avinashbhujan/Encrypter.git</t>
-    </r>
-  </si>
-  <si>
-    <t>change to cloned folder which is the repository</t>
-  </si>
-  <si>
-    <t>Requirement met .  Collaboration can begin</t>
-  </si>
-  <si>
-    <t>Requirement met .  New test aded.  Committed. User G could get an update on his local repo</t>
-  </si>
-  <si>
-    <t>Note: to know which files have changed</t>
+      <t xml:space="preserve">git add </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MessageEncrypter.Tests/UnitTest1.cs</t>
+    </r>
   </si>
   <si>
     <r>
@@ -379,20 +379,111 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">git add </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>MessageEncrypter.Tests/UnitTest1.cs</t>
-    </r>
-  </si>
-  <si>
+      <t xml:space="preserve"> git commit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -m "Added new Test Method"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git push -u </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Encrypter master</t>
+    </r>
+  </si>
+  <si>
+    <t>User S has added another test.</t>
+  </si>
+  <si>
+    <t>git pull</t>
+  </si>
+  <si>
+    <t>Note: Should see 2 commits (hence, 2 SHA1s)</t>
+  </si>
+  <si>
+    <t>git diff HEAD~1</t>
+  </si>
+  <si>
+    <t>User S added changes but needs to revert in the middle of the process</t>
+  </si>
+  <si>
+    <t>Req#</t>
+  </si>
+  <si>
+    <t>User S has been given a new urgent feature to accomplish. He needs to skip the main project and begin the new feature then merge the new feature into the main project.</t>
+  </si>
+  <si>
+    <t>touch newFeature.cs</t>
+  </si>
+  <si>
+    <t>Note: User S adds all codes for the new feature in his editor then saves the file.</t>
+  </si>
+  <si>
+    <t>git branch newBranch</t>
+  </si>
+  <si>
+    <t>git checkout newBranch</t>
+  </si>
+  <si>
+    <t>git checkout master</t>
+  </si>
+  <si>
+    <t>git merge newBranch</t>
+  </si>
+  <si>
+    <t>User S needs to use WinMerge Tool to view differences in file versions.</t>
+  </si>
+  <si>
+    <t>git config diff.tool winmerge</t>
+  </si>
+  <si>
+    <t>Note: User S need to make sure that WinMerge is installed</t>
+  </si>
+  <si>
+    <t>Note: User S makes changes to some files in the working directory, then commits them all</t>
+  </si>
+  <si>
+    <t>git difftool HEAD HEAD~1 newClass.cs</t>
+  </si>
+  <si>
+    <t>Note : User S only wants to see the differences in the newClass.cs file</t>
+  </si>
+  <si>
+    <t>Note: the switch -u comes in handy such that it does not ask for repository name and branch again.</t>
+  </si>
+  <si>
+    <t>Requirement met .  New test added.  Committed. User G could get an update on his local repo</t>
+  </si>
+  <si>
+    <t>User G provided feedback that using VS, he saw too little number of unit tests.  User S should add another test and commit.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">User S </t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -402,122 +493,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> git commit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> -m "Added new Test Method"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">git push -u </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Encrypter master</t>
-    </r>
-  </si>
-  <si>
-    <t>User S has added another test.</t>
-  </si>
-  <si>
-    <t>git pull</t>
-  </si>
-  <si>
-    <t>Note: Should see 2 commits (hence, 2 SHA1s)</t>
-  </si>
-  <si>
-    <t>git diff HEAD~1</t>
-  </si>
-  <si>
-    <t>User S added changes but needs to revert in the middle of the process</t>
-  </si>
-  <si>
-    <t>Req#</t>
-  </si>
-  <si>
-    <t>User S has been given a new urgent feature to accomplish. He needs to skip the main project and begin the new feature then merge the new feature into the main project.</t>
-  </si>
-  <si>
-    <t>touch newFeature.cs</t>
-  </si>
-  <si>
-    <t>Note: User S adds all codes for the new feature in his editor then saves the file.</t>
-  </si>
-  <si>
-    <t>git branch newBranch</t>
-  </si>
-  <si>
-    <t>git checkout newBranch</t>
-  </si>
-  <si>
-    <t>git checkout master</t>
-  </si>
-  <si>
-    <t>git merge newBranch</t>
-  </si>
-  <si>
-    <t>User S needs to use WinMerge Tool to view differences in file versions.</t>
-  </si>
-  <si>
-    <t>git config diff.tool winmerge</t>
-  </si>
-  <si>
-    <t>Note: User S need to make sure that WinMerge is installed</t>
-  </si>
-  <si>
-    <t>Note: User S makes changes to some files in the working directory, then commits them all</t>
-  </si>
-  <si>
-    <t>git difftool HEAD HEAD~1 newClass.cs</t>
-  </si>
-  <si>
-    <t>Note : User S only wants to see the differences in the newClass.cs file</t>
-  </si>
-  <si>
-    <t>Note: the switch -u comes in handy such that it does not ask for repository name and branch again.</t>
-  </si>
-  <si>
-    <t>Requirement met .  New test added.  Committed. User G could get an update on his local repo</t>
-  </si>
-  <si>
-    <t>User G provided feedback that using VS, he saw too little number of unit tests.  User S should add another test and commit.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">User S </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>has the solution "Encrypter" on his Machine.  Created long back. Both of them now need to collaborate.  He needs to setup a local and remote repo for this to happen.  When Setup is done, User G can then pull the repository and work on it.</t>
     </r>
+  </si>
+  <si>
+    <t>git commit</t>
+  </si>
+  <si>
+    <t>Note: A window will appear asking you to enter a commit description.</t>
+  </si>
+  <si>
+    <t>Enter a commit description</t>
   </si>
 </sst>
 </file>
@@ -987,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1006,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -1062,7 +1048,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1123,66 +1109,73 @@
       <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>24</v>
+        <v>62</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="5" t="s">
+    <row r="23" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>1</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
-        <v>1</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1208,6 +1201,7 @@
     <row r="47" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1249,13 +1243,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
@@ -1265,42 +1259,42 @@
     <row r="4" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1308,7 +1302,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1440,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -1459,42 +1453,42 @@
     <row r="4" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1502,7 +1496,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1623,7 +1617,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
@@ -1640,37 +1634,37 @@
         <v>4</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="17"/>
       <c r="C3" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
@@ -1701,7 +1695,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
@@ -1718,23 +1712,23 @@
         <v>5</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="22" customFormat="1" ht="48" x14ac:dyDescent="0.45">
       <c r="A3" s="23"/>
       <c r="B3" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" s="22" customFormat="1" ht="63" x14ac:dyDescent="0.45">
       <c r="A4" s="23"/>
       <c r="B4" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>13</v>
@@ -1744,10 +1738,10 @@
     <row r="5" spans="1:4" s="22" customFormat="1" ht="48" x14ac:dyDescent="0.45">
       <c r="A5" s="23"/>
       <c r="B5" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="23"/>
     </row>

</xml_diff>

<commit_message>
Updated Walkthrough with commit description
</commit_message>
<xml_diff>
--- a/Walkthrough.xlsx
+++ b/Walkthrough.xlsx
@@ -500,10 +500,10 @@
     <t>git commit</t>
   </si>
   <si>
-    <t>Note: A window will appear asking you to enter a commit description.</t>
-  </si>
-  <si>
-    <t>Enter a commit description</t>
+    <t>Note: A window will appear asking you to enter a commit message.</t>
+  </si>
+  <si>
+    <t>Enter a commit message</t>
   </si>
 </sst>
 </file>

</xml_diff>